<commit_message>
Crud Table as of 3/26/2018
Crud Table after updating 3/26/2018 at 9:30pm
</commit_message>
<xml_diff>
--- a/Milestone7/crud.table.xlsx
+++ b/Milestone7/crud.table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Desktop\School\Spring 18\ISQA 4120\Milestone 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>Elementary Process</t>
   </si>
@@ -62,12 +62,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Main Menu</t>
-  </si>
-  <si>
-    <t>Forms Menu</t>
-  </si>
-  <si>
     <t>Vendor Form</t>
   </si>
   <si>
@@ -86,18 +80,9 @@
     <t>Invoice Form</t>
   </si>
   <si>
-    <t>Reports Menu</t>
-  </si>
-  <si>
     <t>Pull-Inventory Form</t>
   </si>
   <si>
-    <t>Inventory Report</t>
-  </si>
-  <si>
-    <t>Invoice Report</t>
-  </si>
-  <si>
     <t>Type Query</t>
   </si>
   <si>
@@ -125,21 +110,9 @@
     <t>Update Pull-Inventory Query</t>
   </si>
   <si>
-    <t>Inventory Report Definition</t>
-  </si>
-  <si>
-    <t>Invoice Report Definition</t>
-  </si>
-  <si>
     <t>Pull-Inventory Report</t>
   </si>
   <si>
-    <t>Pull-Inventory Report Definition</t>
-  </si>
-  <si>
-    <t>App</t>
-  </si>
-  <si>
     <t>Invoice Report Query</t>
   </si>
   <si>
@@ -149,7 +122,7 @@
     <t>U</t>
   </si>
   <si>
-    <t>C</t>
+    <t>CU</t>
   </si>
 </sst>
 </file>
@@ -516,11 +489,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,356 +542,192 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" t="s">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" t="s">
-        <v>41</v>
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" t="s">
-        <v>41</v>
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" t="s">
-        <v>40</v>
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" t="s">
-        <v>40</v>
+        <v>25</v>
+      </c>
+      <c r="K17" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" t="s">
-        <v>41</v>
+        <v>26</v>
+      </c>
+      <c r="I18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" t="s">
-        <v>41</v>
+        <v>27</v>
+      </c>
+      <c r="H19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
+        <v>28</v>
+      </c>
+      <c r="I21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="K24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
         <v>31</v>
       </c>
-      <c r="I25" t="s">
-        <v>41</v>
-      </c>
-      <c r="J25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" t="s">
-        <v>40</v>
-      </c>
-      <c r="J26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="I30" t="s">
-        <v>40</v>
-      </c>
-      <c r="J30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I31" t="s">
-        <v>40</v>
-      </c>
-      <c r="J31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="I32" t="s">
-        <v>39</v>
-      </c>
-      <c r="J32" t="s">
-        <v>39</v>
+      <c r="I22" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>